<commit_message>
.netcore final demo modifications
</commit_message>
<xml_diff>
--- a/DailyWorkReport.xlsx
+++ b/DailyWorkReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934E419F-EC5A-4785-BC5C-F777536EBBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F78BE83-B60C-4C3B-A659-0267C435173B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="1470" windowWidth="21615" windowHeight="14130" xr2:uid="{D08360DC-A95C-4AA3-9766-44BAE5CA1820}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{D08360DC-A95C-4AA3-9766-44BAE5CA1820}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="70">
   <si>
     <t>Domm</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>Editing</t>
+  </si>
+  <si>
+    <t>Grouping</t>
+  </si>
+  <si>
+    <t>Filtering</t>
   </si>
 </sst>
 </file>
@@ -613,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CFBBF5-4962-479C-A8E1-4B1FB2501AF1}">
-  <dimension ref="A1:H246"/>
+  <dimension ref="A1:H261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="D247" sqref="A240:D247"/>
+    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="H260" sqref="H260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2901,6 +2907,150 @@
         <v>8</v>
       </c>
     </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" s="2">
+        <v>45712</v>
+      </c>
+      <c r="B248" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C248" s="3"/>
+      <c r="D248" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" s="2"/>
+      <c r="B249" t="s">
+        <v>1</v>
+      </c>
+      <c r="C249" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D249" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" s="3"/>
+      <c r="B250" s="3"/>
+      <c r="C250" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D250" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" s="3"/>
+      <c r="B251" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C251" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D251" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" s="3"/>
+      <c r="B252" s="3"/>
+      <c r="C252" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D252" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" s="3"/>
+      <c r="B253" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C253" s="3"/>
+      <c r="D253" s="4">
+        <f>SUM(D247:D252)</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" s="2">
+        <v>45713</v>
+      </c>
+      <c r="B255" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C255" s="3"/>
+      <c r="D255" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" s="2"/>
+      <c r="B256" t="s">
+        <v>1</v>
+      </c>
+      <c r="C256" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D256" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="3"/>
+      <c r="B257" s="3"/>
+      <c r="C257" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D257" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" s="3"/>
+      <c r="B258" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C258" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D258" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" s="3"/>
+      <c r="B259" s="3"/>
+      <c r="C259" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D259" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" s="3"/>
+      <c r="B260" s="3"/>
+      <c r="C260" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D260" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="3"/>
+      <c r="B261" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C261" s="3"/>
+      <c r="D261" s="4">
+        <f>SUM(D254:D260)</f>
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
Extra changes into checkbox and datebox editors
</commit_message>
<xml_diff>
--- a/DailyWorkReport.xlsx
+++ b/DailyWorkReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E4E1FC-03E0-4C77-BCB4-CAAEEB9671F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C156BC93-7594-43A3-9615-78BB0A146A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{D08360DC-A95C-4AA3-9766-44BAE5CA1820}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21615" windowHeight="14130" xr2:uid="{D08360DC-A95C-4AA3-9766-44BAE5CA1820}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -667,7 +667,7 @@
   <dimension ref="A1:H309"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
-      <selection activeCell="I308" sqref="I308"/>
+      <selection activeCell="N290" sqref="N290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Project changes and add caching
</commit_message>
<xml_diff>
--- a/DailyWorkReport.xlsx
+++ b/DailyWorkReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hina.j\source\repos\RKIT_Internship_work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD0458A-AE4F-4381-A006-7D2455BD4F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B5C800-78A5-4092-9472-EAE78CD6D6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D08360DC-A95C-4AA3-9766-44BAE5CA1820}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21615" windowHeight="14130" xr2:uid="{D08360DC-A95C-4AA3-9766-44BAE5CA1820}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="98">
   <si>
     <t>Domm</t>
   </si>
@@ -301,6 +301,24 @@
   </si>
   <si>
     <t xml:space="preserve">Operational Training Practice </t>
+  </si>
+  <si>
+    <t>Operational Training Reconsile</t>
+  </si>
+  <si>
+    <t>Redis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM API Training + Discussion </t>
+  </si>
+  <si>
+    <t>Read React Documentation</t>
+  </si>
+  <si>
+    <t>DevExtreme Project changes</t>
+  </si>
+  <si>
+    <t>DevExtreme Documentation</t>
   </si>
 </sst>
 </file>
@@ -685,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CFBBF5-4962-479C-A8E1-4B1FB2501AF1}">
-  <dimension ref="A1:H352"/>
+  <dimension ref="A1:H368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
-      <selection activeCell="D353" sqref="A345:D353"/>
+    <sheetView tabSelected="1" topLeftCell="A345" workbookViewId="0">
+      <selection activeCell="D369" sqref="A362:D369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3972,6 +3990,156 @@
         <v>8</v>
       </c>
     </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A354" s="2">
+        <v>45729</v>
+      </c>
+      <c r="B354" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C354" s="3"/>
+      <c r="D354" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B355" t="s">
+        <v>1</v>
+      </c>
+      <c r="C355" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D355" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A356" s="2"/>
+      <c r="C356" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D356" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A357" s="3"/>
+      <c r="B357" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C357" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D357" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A358" s="3"/>
+      <c r="B358" s="3"/>
+      <c r="C358" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D358" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A359" s="3"/>
+      <c r="B359" s="3"/>
+      <c r="C359" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D359" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A360" s="3"/>
+      <c r="B360" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C360" s="3"/>
+      <c r="D360" s="4">
+        <f>SUM(D353:D359)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A362" s="2">
+        <v>45733</v>
+      </c>
+      <c r="B362" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C362" s="3"/>
+      <c r="D362" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B363" t="s">
+        <v>1</v>
+      </c>
+      <c r="C363" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D363" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A364" s="2"/>
+      <c r="C364" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D364" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A365" s="3"/>
+      <c r="B365" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C365" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D365" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A366" s="3"/>
+      <c r="B366" s="3"/>
+      <c r="C366" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D366" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A367" s="3"/>
+      <c r="B367" s="3"/>
+      <c r="C367" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D367" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A368" s="3"/>
+      <c r="B368" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C368" s="3"/>
+      <c r="D368" s="4">
+        <f>SUM(D361:D367)</f>
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>